<commit_message>
Updated price of Labyrinth
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -433,7 +433,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,14 +467,14 @@
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>12.21</v>
+        <v>20.16</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <f>D2*C2</f>
-        <v>12.21</v>
+        <f t="shared" ref="E2:E9" si="0">D2*C2</f>
+        <v>20.16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="2">
-        <f>D3*C3</f>
+        <f t="shared" si="0"/>
         <v>24.42</v>
       </c>
     </row>
@@ -509,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f>D4*C4</f>
+        <f t="shared" si="0"/>
         <v>3.63</v>
       </c>
     </row>
@@ -527,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f>D5*C5</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
     </row>
@@ -545,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="2">
-        <f>D6*C6</f>
+        <f t="shared" si="0"/>
         <v>25.98</v>
       </c>
     </row>
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <f>D7*C7</f>
+        <f t="shared" si="0"/>
         <v>49.99</v>
       </c>
     </row>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <f>D8*C8</f>
+        <f t="shared" si="0"/>
         <v>19.989999999999998</v>
       </c>
     </row>
@@ -599,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f>D9*C9</f>
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="E13" s="2">
         <f>SUM(E2:E9)</f>
-        <v>236.12</v>
+        <v>244.07000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>